<commit_message>
reconcile scenarios w/ and w/o ERC cap
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -2599,7 +2599,7 @@
   <dimension ref="A4:AE29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D13" sqref="D13:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2912,7 +2912,7 @@
         <v>40</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -3004,7 +3004,7 @@
         <v>40</v>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -3096,7 +3096,7 @@
         <v>40</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -3188,7 +3188,7 @@
         <v>40</v>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -3375,7 +3375,7 @@
         <v>40</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
@@ -3467,7 +3467,7 @@
         <v>40</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
@@ -3559,7 +3559,7 @@
         <v>40</v>
       </c>
       <c r="D16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
@@ -3651,7 +3651,7 @@
         <v>40</v>
       </c>
       <c r="D17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
@@ -4477,7 +4477,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>